<commit_message>
employee information management MOCK UI
</commit_message>
<xml_diff>
--- a/rc-eims/Integrate Adding Employee feature in the Employee System Test case.xlsx
+++ b/rc-eims/Integrate Adding Employee feature in the Employee System Test case.xlsx
@@ -1,32 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D283020F-3C27-4C1B-85D6-FEA5371640D6}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="6810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -189,13 +172,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;₱&quot;* #,##0_-;\-&quot;₱&quot;* #,##0_-;_-&quot;₱&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,7 +192,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -212,8 +201,159 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +372,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -243,29 +569,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -273,29 +599,271 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -339,17 +907,61 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -398,7 +1010,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -431,26 +1043,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -483,23 +1078,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -641,30 +1219,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="29.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="27.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="24.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="31.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -723,7 +1296,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="84" customHeight="1">
+    <row r="5" ht="84" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -737,7 +1310,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="31.5" customHeight="1">
+    <row r="6" ht="31.5" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -787,7 +1360,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="259.5">
+    <row r="9" ht="105" spans="1:8">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -947,7 +1520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="321">
+    <row r="20" ht="120" spans="1:8">
       <c r="A20" s="9">
         <v>2</v>
       </c>
@@ -1107,7 +1680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="409.6">
+    <row r="31" ht="195" spans="1:8">
       <c r="A31" s="9">
         <v>3</v>
       </c>
@@ -1267,7 +1840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="244.5">
+    <row r="42" ht="90" spans="1:8">
       <c r="A42" s="9">
         <v>4</v>
       </c>
@@ -1289,31 +1862,32 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
     <mergeCell ref="B34:H34"/>
     <mergeCell ref="B35:H35"/>
     <mergeCell ref="B36:H36"/>
     <mergeCell ref="B37:H37"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>